<commit_message>
new response model class added
</commit_message>
<xml_diff>
--- a/src/test/resources/DemoData.xlsx
+++ b/src/test/resources/DemoData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\DemoRestAssuredWithCucumber\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A8093-4475-4198-8B57-811761DA4A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC96CD39-354A-4A4A-B198-E5F6CD67C99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Testcases</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Data4</t>
+  </si>
+  <si>
+    <t>ghdbjkm</t>
+  </si>
+  <si>
+    <t>cgfvhbjnk</t>
   </si>
 </sst>
 </file>
@@ -417,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,8 +484,8 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>10</v>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -492,8 +498,8 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -505,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6197F818-179D-4DB8-9271-20D487307F37}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>